<commit_message>
Test Cases for lab06 - Ethan
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/lab6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eadch\PycharmProjects\cs151-lab6-ethan-andrew-lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D46B02-26E9-E948-BF2B-078F7C3B7399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E3FCD2-F93B-4F9F-AEB4-446D8B659542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -34,86 +34,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Test number</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>normal deposit</t>
-  </si>
-  <si>
-    <t>normal withdrawal</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> view balance</t>
-  </si>
-  <si>
-    <t>higher withdrawl</t>
-  </si>
-  <si>
-    <t>in: amount</t>
-  </si>
-  <si>
-    <t>out: balance</t>
-  </si>
-  <si>
-    <t>initial balance</t>
-  </si>
-  <si>
-    <t>in: coice</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>proper exit</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>do you want to use atm again</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Thank you</t>
-  </si>
-  <si>
-    <t>deposit negative</t>
-  </si>
-  <si>
-    <t>out: menu</t>
-  </si>
-  <si>
-    <t>negative balance</t>
-  </si>
-  <si>
-    <t>out: info</t>
-  </si>
-  <si>
-    <t>negative number</t>
-  </si>
-  <si>
-    <t>withdraw negative</t>
+    <t>Valid Deposit</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Deposit successful! Your new balance is $1500.00.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Menu Option	</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Error: Invalid choice. Please enter D, W, V, or E.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Withdrawal	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Withdrawal successful! Your new balance is $800.00.	</t>
+  </si>
+  <si>
+    <t>Exit Program</t>
+  </si>
+  <si>
+    <t>Thank you for using the ATM program. Goodbye!</t>
+  </si>
+  <si>
+    <t>Withdrawal Leading to Negative Balance</t>
+  </si>
+  <si>
+    <t>Withdrawal successful! Your new balance is -$100.00. Warning: You have a negative balance. You will be charged 5% interest.</t>
+  </si>
+  <si>
+    <t>Non-numeric Input for Deposit or Withdrawal</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Error: Please enter a valid number.</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,8 +134,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -307,7 +321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,211 +471,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127005B9-9F5E-0446-B242-2658EACB013E}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="47.625" customWidth="1"/>
+    <col min="3" max="3" width="21.125" customWidth="1"/>
+    <col min="4" max="4" width="87.5" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
+    <col min="7" max="7" width="33.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>500</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C4" s="2">
+        <v>200</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1100</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <f>1100</f>
-        <v>1100</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>800</v>
-      </c>
-      <c r="E3">
-        <v>1800</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>1000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1200</v>
-      </c>
-      <c r="E5">
-        <v>-200</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>-100</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>-100</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16">
-        <v>1000</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>